<commit_message>
Added disasters dataset, fixed bilateral fixed effects dummies, fixed the migration database, added migration rates.
</commit_message>
<xml_diff>
--- a/Data/Migration.xlsx
+++ b/Data/Migration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Desktop\Dissertation\Migration\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397039E9-6A77-40EE-B35E-1A316734012C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E246BAA-9F5A-46D9-A66A-0B8E1651FE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="12645" xr2:uid="{E6E3DD21-C52D-426C-9B93-90E17570CD3F}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{E6E3DD21-C52D-426C-9B93-90E17570CD3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$2755</definedName>
     <definedName name="MyData">Sheet1!$D$14:$O$20</definedName>
     <definedName name="MyData2">'[1]Table 1'!$Z$4:$AO$19</definedName>
     <definedName name="s">Sheet1!$D$5:$R$21</definedName>
@@ -1353,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CCE975-9AF9-40CE-9B57-B9B7C685523F}">
   <dimension ref="A1:V2755"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1436" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C467" sqref="C467"/>
+    <sheetView tabSelected="1" topLeftCell="A2703" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F497" sqref="F497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11355,7 +11356,7 @@
         <v>0</v>
       </c>
       <c r="C714" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D714">
         <v>1.2</v>
@@ -11369,7 +11370,7 @@
         <v>0</v>
       </c>
       <c r="C715" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D715">
         <v>1.5</v>
@@ -11383,7 +11384,7 @@
         <v>0</v>
       </c>
       <c r="C716" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D716">
         <v>0.1</v>
@@ -11397,7 +11398,7 @@
         <v>0</v>
       </c>
       <c r="C717" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D717">
         <v>8</v>
@@ -11411,7 +11412,7 @@
         <v>0</v>
       </c>
       <c r="C718" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D718">
         <v>0.6</v>
@@ -11425,7 +11426,7 @@
         <v>0</v>
       </c>
       <c r="C719" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D719">
         <v>1</v>
@@ -11439,7 +11440,7 @@
         <v>0</v>
       </c>
       <c r="C720" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D720">
         <v>0.5</v>
@@ -11579,7 +11580,7 @@
         <v>1</v>
       </c>
       <c r="C730" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D730">
         <v>5.7</v>
@@ -11593,7 +11594,7 @@
         <v>1</v>
       </c>
       <c r="C731" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D731">
         <v>2</v>
@@ -11607,7 +11608,7 @@
         <v>1</v>
       </c>
       <c r="C732" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D732">
         <v>0.5</v>
@@ -11621,7 +11622,7 @@
         <v>1</v>
       </c>
       <c r="C733" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D733">
         <v>3.6</v>
@@ -11635,7 +11636,7 @@
         <v>1</v>
       </c>
       <c r="C734" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D734">
         <v>0.1</v>
@@ -11649,7 +11650,7 @@
         <v>1</v>
       </c>
       <c r="C735" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D735">
         <v>0.6</v>
@@ -11663,7 +11664,7 @@
         <v>1</v>
       </c>
       <c r="C736" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D736">
         <v>0.7</v>
@@ -11803,7 +11804,7 @@
         <v>2</v>
       </c>
       <c r="C746" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D746">
         <v>0.3</v>
@@ -11817,7 +11818,7 @@
         <v>2</v>
       </c>
       <c r="C747" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D747">
         <v>0.8</v>
@@ -11831,7 +11832,7 @@
         <v>2</v>
       </c>
       <c r="C748" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D748">
         <v>0.1</v>
@@ -11845,7 +11846,7 @@
         <v>2</v>
       </c>
       <c r="C749" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D749">
         <v>1.8</v>
@@ -11859,7 +11860,7 @@
         <v>2</v>
       </c>
       <c r="C750" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D750">
         <v>1.7</v>
@@ -11873,7 +11874,7 @@
         <v>2</v>
       </c>
       <c r="C751" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D751">
         <v>0.1</v>
@@ -11887,7 +11888,7 @@
         <v>2</v>
       </c>
       <c r="C752" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D752">
         <v>0.1</v>
@@ -12027,7 +12028,7 @@
         <v>3</v>
       </c>
       <c r="C762" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D762">
         <v>0</v>
@@ -12041,7 +12042,7 @@
         <v>3</v>
       </c>
       <c r="C763" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D763">
         <v>0.2</v>
@@ -12055,7 +12056,7 @@
         <v>3</v>
       </c>
       <c r="C764" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D764">
         <v>0</v>
@@ -12069,7 +12070,7 @@
         <v>3</v>
       </c>
       <c r="C765" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D765">
         <v>0.3</v>
@@ -12083,7 +12084,7 @@
         <v>3</v>
       </c>
       <c r="C766" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D766">
         <v>0</v>
@@ -12097,7 +12098,7 @@
         <v>3</v>
       </c>
       <c r="C767" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D767">
         <v>0</v>
@@ -12111,7 +12112,7 @@
         <v>3</v>
       </c>
       <c r="C768" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D768">
         <v>1.6</v>
@@ -12251,7 +12252,7 @@
         <v>4</v>
       </c>
       <c r="C778" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D778">
         <v>1.1000000000000001</v>
@@ -12265,7 +12266,7 @@
         <v>4</v>
       </c>
       <c r="C779" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D779">
         <v>0.4</v>
@@ -12279,7 +12280,7 @@
         <v>4</v>
       </c>
       <c r="C780" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D780">
         <v>0.1</v>
@@ -12293,7 +12294,7 @@
         <v>4</v>
       </c>
       <c r="C781" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D781">
         <v>4.4000000000000004</v>
@@ -12307,7 +12308,7 @@
         <v>4</v>
       </c>
       <c r="C782" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D782">
         <v>0.1</v>
@@ -12321,7 +12322,7 @@
         <v>4</v>
       </c>
       <c r="C783" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D783">
         <v>0.3</v>
@@ -12335,7 +12336,7 @@
         <v>4</v>
       </c>
       <c r="C784" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D784">
         <v>0.6</v>
@@ -12475,7 +12476,7 @@
         <v>5</v>
       </c>
       <c r="C794" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D794">
         <v>0.4</v>
@@ -12489,7 +12490,7 @@
         <v>5</v>
       </c>
       <c r="C795" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D795">
         <v>0.6</v>
@@ -12503,7 +12504,7 @@
         <v>5</v>
       </c>
       <c r="C796" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D796">
         <v>0.1</v>
@@ -12517,7 +12518,7 @@
         <v>5</v>
       </c>
       <c r="C797" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D797">
         <v>3.4</v>
@@ -12531,7 +12532,7 @@
         <v>5</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D798">
         <v>1.5</v>
@@ -12545,7 +12546,7 @@
         <v>5</v>
       </c>
       <c r="C799" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D799">
         <v>0.7</v>
@@ -12559,7 +12560,7 @@
         <v>5</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D800">
         <v>1.3</v>
@@ -12699,7 +12700,7 @@
         <v>6</v>
       </c>
       <c r="C810" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D810">
         <v>3.3</v>
@@ -12713,7 +12714,7 @@
         <v>6</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D811">
         <v>25</v>
@@ -12727,7 +12728,7 @@
         <v>6</v>
       </c>
       <c r="C812" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D812">
         <v>0.2</v>
@@ -12741,7 +12742,7 @@
         <v>6</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D813">
         <v>5.6</v>
@@ -12755,7 +12756,7 @@
         <v>6</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D814">
         <v>0.1</v>
@@ -12769,7 +12770,7 @@
         <v>6</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D815">
         <v>0.8</v>
@@ -12783,7 +12784,7 @@
         <v>6</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D816">
         <v>0.5</v>
@@ -12923,7 +12924,7 @@
         <v>7</v>
       </c>
       <c r="C826" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D826">
         <v>1.8</v>
@@ -12937,7 +12938,7 @@
         <v>7</v>
       </c>
       <c r="C827" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D827">
         <v>0.8</v>
@@ -12951,7 +12952,7 @@
         <v>7</v>
       </c>
       <c r="C828" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D828">
         <v>1.9</v>
@@ -12965,7 +12966,7 @@
         <v>7</v>
       </c>
       <c r="C829" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D829">
         <v>0.8</v>
@@ -12979,7 +12980,7 @@
         <v>7</v>
       </c>
       <c r="C830" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D830">
         <v>0</v>
@@ -12993,7 +12994,7 @@
         <v>7</v>
       </c>
       <c r="C831" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D831">
         <v>0</v>
@@ -13007,7 +13008,7 @@
         <v>7</v>
       </c>
       <c r="C832" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D832">
         <v>0</v>
@@ -13147,7 +13148,7 @@
         <v>8</v>
       </c>
       <c r="C842" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D842">
         <v>42.4</v>
@@ -13161,7 +13162,7 @@
         <v>8</v>
       </c>
       <c r="C843" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D843">
         <v>0.7</v>
@@ -13175,7 +13176,7 @@
         <v>8</v>
       </c>
       <c r="C844" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D844">
         <v>0.6</v>
@@ -13189,7 +13190,7 @@
         <v>8</v>
       </c>
       <c r="C845" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D845">
         <v>4.0999999999999996</v>
@@ -13203,7 +13204,7 @@
         <v>8</v>
       </c>
       <c r="C846" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D846">
         <v>0.1</v>
@@ -13217,7 +13218,7 @@
         <v>8</v>
       </c>
       <c r="C847" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D847">
         <v>0.1</v>
@@ -13231,7 +13232,7 @@
         <v>8</v>
       </c>
       <c r="C848" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D848">
         <v>0</v>
@@ -13371,7 +13372,7 @@
         <v>9</v>
       </c>
       <c r="C858" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D858">
         <v>0.1</v>
@@ -13385,7 +13386,7 @@
         <v>9</v>
       </c>
       <c r="C859" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D859">
         <v>0.4</v>
@@ -13399,7 +13400,7 @@
         <v>9</v>
       </c>
       <c r="C860" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D860">
         <v>0</v>
@@ -13413,7 +13414,7 @@
         <v>9</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D861">
         <v>5.9</v>
@@ -13427,7 +13428,7 @@
         <v>9</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D862">
         <v>0.1</v>
@@ -13441,7 +13442,7 @@
         <v>9</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D863">
         <v>93.4</v>
@@ -13455,7 +13456,7 @@
         <v>9</v>
       </c>
       <c r="C864" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D864">
         <v>3.1</v>
@@ -13595,7 +13596,7 @@
         <v>10</v>
       </c>
       <c r="C874" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D874">
         <v>0.7</v>
@@ -13609,7 +13610,7 @@
         <v>10</v>
       </c>
       <c r="C875" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D875">
         <v>1.3</v>
@@ -13623,7 +13624,7 @@
         <v>10</v>
       </c>
       <c r="C876" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D876">
         <v>0</v>
@@ -13637,7 +13638,7 @@
         <v>10</v>
       </c>
       <c r="C877" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D877">
         <v>1.6</v>
@@ -13651,7 +13652,7 @@
         <v>10</v>
       </c>
       <c r="C878" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D878">
         <v>0</v>
@@ -13665,7 +13666,7 @@
         <v>10</v>
       </c>
       <c r="C879" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D879">
         <v>2.7</v>
@@ -13679,7 +13680,7 @@
         <v>10</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D880">
         <v>35.799999999999997</v>
@@ -13819,7 +13820,7 @@
         <v>11</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D890">
         <v>1.2</v>
@@ -13833,7 +13834,7 @@
         <v>11</v>
       </c>
       <c r="C891" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D891">
         <v>4.9000000000000004</v>
@@ -13847,7 +13848,7 @@
         <v>11</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D892">
         <v>0.5</v>
@@ -13861,7 +13862,7 @@
         <v>11</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D893">
         <v>103.8</v>
@@ -13875,7 +13876,7 @@
         <v>11</v>
       </c>
       <c r="C894" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D894">
         <v>1.3</v>
@@ -13889,7 +13890,7 @@
         <v>11</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D895">
         <v>1.5</v>
@@ -13903,7 +13904,7 @@
         <v>11</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D896">
         <v>2.8</v>
@@ -14043,7 +14044,7 @@
         <v>12</v>
       </c>
       <c r="C906" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D906">
         <v>0.1</v>
@@ -14057,7 +14058,7 @@
         <v>12</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D907">
         <v>0.3</v>
@@ -14071,7 +14072,7 @@
         <v>12</v>
       </c>
       <c r="C908" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D908">
         <v>0.1</v>
@@ -14085,7 +14086,7 @@
         <v>12</v>
       </c>
       <c r="C909" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D909">
         <v>0</v>
@@ -14099,7 +14100,7 @@
         <v>12</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D910">
         <v>7.4</v>
@@ -14113,7 +14114,7 @@
         <v>12</v>
       </c>
       <c r="C911" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D911">
         <v>0.3</v>
@@ -14127,7 +14128,7 @@
         <v>12</v>
       </c>
       <c r="C912" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D912">
         <v>0.7</v>
@@ -14267,7 +14268,7 @@
         <v>18</v>
       </c>
       <c r="C922" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D922">
         <v>2.5</v>
@@ -14281,7 +14282,7 @@
         <v>18</v>
       </c>
       <c r="C923" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D923">
         <v>0.7</v>
@@ -14295,7 +14296,7 @@
         <v>18</v>
       </c>
       <c r="C924" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D924">
         <v>0.1</v>
@@ -14309,7 +14310,7 @@
         <v>18</v>
       </c>
       <c r="C925" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D925">
         <v>9</v>
@@ -14323,7 +14324,7 @@
         <v>18</v>
       </c>
       <c r="C926" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D926">
         <v>0.8</v>
@@ -14337,7 +14338,7 @@
         <v>18</v>
       </c>
       <c r="C927" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D927">
         <v>1.7</v>
@@ -14351,7 +14352,7 @@
         <v>18</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D928">
         <v>0.4</v>
@@ -14491,7 +14492,7 @@
         <v>17</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D938">
         <v>0</v>
@@ -14505,7 +14506,7 @@
         <v>17</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D939">
         <v>0</v>
@@ -14519,7 +14520,7 @@
         <v>17</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D940">
         <v>0</v>
@@ -14533,7 +14534,7 @@
         <v>17</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D941">
         <v>0</v>
@@ -14547,7 +14548,7 @@
         <v>17</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D942">
         <v>0</v>
@@ -14561,7 +14562,7 @@
         <v>17</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D943">
         <v>0.5</v>
@@ -14575,7 +14576,7 @@
         <v>17</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D944">
         <v>0.6</v>
@@ -14715,7 +14716,7 @@
         <v>19</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D954">
         <v>0</v>
@@ -14729,7 +14730,7 @@
         <v>19</v>
       </c>
       <c r="C955" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D955">
         <v>0</v>
@@ -14743,7 +14744,7 @@
         <v>19</v>
       </c>
       <c r="C956" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D956">
         <v>0</v>
@@ -14757,7 +14758,7 @@
         <v>19</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D957">
         <v>2.2000000000000002</v>
@@ -14771,7 +14772,7 @@
         <v>19</v>
       </c>
       <c r="C958" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D958">
         <v>0.1</v>
@@ -14785,7 +14786,7 @@
         <v>19</v>
       </c>
       <c r="C959" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D959">
         <v>1.4</v>
@@ -14799,7 +14800,7 @@
         <v>19</v>
       </c>
       <c r="C960" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D960">
         <v>0</v>
@@ -40448,6 +40449,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D2755" xr:uid="{62CCE975-9AF9-40CE-9B57-B9B7C685523F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>